<commit_message>
Final commit Project Buffalocart
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageTitle" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,22 @@
     <sheet name="HomePageTitle" sheetId="8" r:id="rId6"/>
     <sheet name="UsersPageTitle" sheetId="12" r:id="rId7"/>
     <sheet name="ListUserManageListUsers" sheetId="13" r:id="rId8"/>
+    <sheet name="UserCreation" sheetId="14" r:id="rId9"/>
+    <sheet name="RolePageTitle" sheetId="16" r:id="rId10"/>
+    <sheet name="AddRolePageTitle" sheetId="17" r:id="rId11"/>
+    <sheet name="EditRolePageTitle" sheetId="18" r:id="rId12"/>
+    <sheet name="SalesCommAgentPageTitle" sheetId="19" r:id="rId13"/>
+    <sheet name="EditUserPageTitle" sheetId="20" r:id="rId14"/>
+    <sheet name="UserPageUserDetails" sheetId="21" r:id="rId15"/>
+    <sheet name="UserPageInvalidData" sheetId="22" r:id="rId16"/>
+    <sheet name="AddUserPageErrormssg" sheetId="23" r:id="rId17"/>
+    <sheet name="AddUsersPageTitle" sheetId="25" r:id="rId18"/>
+    <sheet name="UserwithInvalidData" sheetId="27" r:id="rId19"/>
+    <sheet name="ViewUserDetails" sheetId="28" r:id="rId20"/>
+    <sheet name="Edit Sales Agent Details" sheetId="29" r:id="rId21"/>
+    <sheet name="Delete Sales Agent" sheetId="30" r:id="rId22"/>
+    <sheet name="SelectRoleFromList" sheetId="31" r:id="rId23"/>
+    <sheet name="DeleteUser" sheetId="32" r:id="rId24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>expected url</t>
   </si>
@@ -80,13 +96,139 @@
   </si>
   <si>
     <t>Sales Commission Agents</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Roles - Lloll</t>
+  </si>
+  <si>
+    <t>Expected title</t>
+  </si>
+  <si>
+    <t>Add Role - Lloll</t>
+  </si>
+  <si>
+    <t>Edit Role - Lloll</t>
+  </si>
+  <si>
+    <t>Sales Commission Agents - Lloll</t>
+  </si>
+  <si>
+    <t>Edit user - Lloll</t>
+  </si>
+  <si>
+    <t>email id</t>
+  </si>
+  <si>
+    <t>xdrij@gmail.com</t>
+  </si>
+  <si>
+    <t>No matching records found</t>
+  </si>
+  <si>
+    <t>expected message</t>
+  </si>
+  <si>
+    <t>Expected Error Message</t>
+  </si>
+  <si>
+    <t>This field is required.</t>
+  </si>
+  <si>
+    <t>Expected Title</t>
+  </si>
+  <si>
+    <t>Add user - Lloll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testerauto</t>
+  </si>
+  <si>
+    <t>tester@1234</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>tester.automation@gmail.com</t>
+  </si>
+  <si>
+    <t>Mrs edwpa yslaw</t>
+  </si>
+  <si>
+    <t>Coordinator</t>
+  </si>
+  <si>
+    <t>ezznz</t>
+  </si>
+  <si>
+    <t>qtofq</t>
+  </si>
+  <si>
+    <t>Mrs sjnke fzlmb</t>
+  </si>
+  <si>
+    <t>Mrs lvohn ynbqi</t>
+  </si>
+  <si>
+    <t>jkpps</t>
+  </si>
+  <si>
+    <t>iswbz@gmail.com</t>
+  </si>
+  <si>
+    <t>gcnwy@gmail.com</t>
+  </si>
+  <si>
+    <t>urihs@gmail.com</t>
+  </si>
+  <si>
+    <t>Expected Details</t>
+  </si>
+  <si>
+    <t>mail id</t>
+  </si>
+  <si>
+    <t>tzypj@gmail.com</t>
+  </si>
+  <si>
+    <t>Sales Agent Details</t>
+  </si>
+  <si>
+    <t>zltha@gmail.com</t>
+  </si>
+  <si>
+    <t>expected_role</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +245,27 @@
     <font>
       <b/>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -124,10 +287,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -136,8 +300,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -442,6 +610,335 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
@@ -476,6 +973,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
@@ -616,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -646,4 +1265,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>